<commit_message>
Alterações na Ordenação dos Tabs
</commit_message>
<xml_diff>
--- a/Arquivos Fornecedores/aldo.xlsx
+++ b/Arquivos Fornecedores/aldo.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colaborador.053\Desktop\TESTE CROSSSYS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7470"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$1662</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -10007,7 +10002,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -10074,7 +10069,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -10082,6 +10077,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda 2" xfId="1"/>
@@ -10144,7 +10140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -10179,7 +10175,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -10356,7 +10352,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10364,10 +10360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1662"/>
+  <dimension ref="A1:G1662"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12149,7 +12145,7 @@
         <v>281.39</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>286</v>
       </c>
@@ -12163,7 +12159,7 @@
         <v>141.26</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>288</v>
       </c>
@@ -12177,7 +12173,7 @@
         <v>141.26</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>290</v>
       </c>
@@ -12191,7 +12187,7 @@
         <v>141.26</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>292</v>
       </c>
@@ -12205,7 +12201,7 @@
         <v>401.18</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>294</v>
       </c>
@@ -12216,10 +12212,16 @@
         <v>10</v>
       </c>
       <c r="E149">
+        <v>555</v>
+      </c>
+      <c r="F149">
         <v>846.42</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G149">
+        <v>946.42</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>296</v>
       </c>
@@ -12229,11 +12231,11 @@
       <c r="D150">
         <v>10</v>
       </c>
-      <c r="E150">
+      <c r="E150" s="5">
         <v>435.08</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>298</v>
       </c>
@@ -12247,7 +12249,7 @@
         <v>65.03</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>300</v>
       </c>
@@ -12261,7 +12263,7 @@
         <v>401.18</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>302</v>
       </c>
@@ -12275,7 +12277,7 @@
         <v>220.37</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>304</v>
       </c>
@@ -12289,7 +12291,7 @@
         <v>819.3</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>306</v>
       </c>
@@ -12303,7 +12305,7 @@
         <v>394.4</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>308</v>
       </c>
@@ -12317,7 +12319,7 @@
         <v>394.4</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>310</v>
       </c>
@@ -12331,7 +12333,7 @@
         <v>211.33</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>312</v>
       </c>
@@ -12342,7 +12344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>314</v>
       </c>
@@ -12353,7 +12355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>316</v>
       </c>
@@ -31178,5 +31180,6 @@
   </sheetData>
   <autoFilter ref="A1:E1662"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>